<commit_message>
Copy Files From Source Repo (2024-11-01 17:14)
</commit_message>
<xml_diff>
--- a/Allfiles/Demo/Data/ManagerCategory.xlsx
+++ b/Allfiles/Demo/Data/ManagerCategory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\educate\courseware\microsoft\moc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsofteur-my.sharepoint.com/personal/v-alisonf_microsoft_com/Documents/Documents/GitHub/afelix-95/PL-300-Microsoft-Power-BI-Data-Analyst/Allfiles/Demo/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5B8F62-8297-422C-B33A-88A55EA73CD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5B8F62-8297-422C-B33A-88A55EA73CD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AA15AE41-7328-4F51-9EFB-379C446C672F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AA15AE41-7328-4F51-9EFB-379C446C672F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -263,9 +263,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -303,7 +303,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -409,7 +409,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -551,7 +551,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -565,14 +565,14 @@
       <selection activeCell="C8" sqref="A1:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="78.7109375" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="78.6640625" customWidth="1"/>
     <col min="3" max="3" width="53" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -583,7 +583,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -594,7 +594,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -605,7 +605,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -616,7 +616,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -627,7 +627,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -638,7 +638,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -649,7 +649,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -669,4 +669,10 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Privileged" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Copy Files From Source Repo (2024-11-01 18:56)
</commit_message>
<xml_diff>
--- a/Allfiles/Demo/Data/ManagerCategory.xlsx
+++ b/Allfiles/Demo/Data/ManagerCategory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\educate\courseware\microsoft\moc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsofteur-my.sharepoint.com/personal/v-alisonf_microsoft_com/Documents/Documents/GitHub/afelix-95/PL-300-Microsoft-Power-BI-Data-Analyst/Allfiles/Demo/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5B8F62-8297-422C-B33A-88A55EA73CD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5B8F62-8297-422C-B33A-88A55EA73CD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AA15AE41-7328-4F51-9EFB-379C446C672F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AA15AE41-7328-4F51-9EFB-379C446C672F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -263,9 +263,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -303,7 +303,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -409,7 +409,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -551,7 +551,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -565,14 +565,14 @@
       <selection activeCell="C8" sqref="A1:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="78.7109375" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="78.6640625" customWidth="1"/>
     <col min="3" max="3" width="53" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -583,7 +583,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -594,7 +594,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -605,7 +605,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -616,7 +616,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -627,7 +627,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -638,7 +638,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -649,7 +649,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -669,4 +669,10 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Privileged" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>